<commit_message>
added rotating pizza, moving bckgrnd
</commit_message>
<xml_diff>
--- a/oceny.xlsx
+++ b/oceny.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\robotki\pizza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A26EEF31-BC8C-A044-ADE4-CCA4F4AADFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12147C8-F557-453B-96DC-6F12C6EA84B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F38ACD07-8556-40BF-8B0A-F3F863780D4E}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" xr2:uid="{F38ACD07-8556-40BF-8B0A-F3F863780D4E}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
   <si>
     <t>Nazwa</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>ogólna opinia</t>
+  </si>
+  <si>
+    <t>kreska mąki</t>
   </si>
 </sst>
 </file>
@@ -487,15 +490,15 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.31640625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,7 +533,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -569,7 +572,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -608,7 +611,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -647,7 +650,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -686,7 +689,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -725,7 +728,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -764,7 +767,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -803,24 +806,46 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="6"/>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3">
+        <v>9</v>
+      </c>
+      <c r="E9" s="6">
+        <v>8</v>
+      </c>
+      <c r="F9" s="3">
+        <v>8</v>
+      </c>
+      <c r="G9" s="6">
+        <v>6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>9</v>
+      </c>
+      <c r="I9" s="6">
+        <v>8.5</v>
+      </c>
+      <c r="J9" s="3">
+        <v>9</v>
+      </c>
+      <c r="K9" s="6">
+        <v>9</v>
+      </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+        <v>84.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="B10" s="3"/>
       <c r="C10" s="6"/>
@@ -837,7 +862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6"/>
@@ -854,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6"/>
@@ -871,7 +896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6"/>
@@ -888,7 +913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="B14" s="3"/>
       <c r="C14" s="6"/>
@@ -905,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="B15" s="3"/>
       <c r="C15" s="6"/>

</xml_diff>